<commit_message>
Added script for creating distributable exe
</commit_message>
<xml_diff>
--- a/samples/NortheastOpportunities_081122 - Copy.xlsx
+++ b/samples/NortheastOpportunities_081122 - Copy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t xml:space="preserve">Opportunity Owner</t>
   </si>
@@ -123,6 +123,18 @@
   <si>
     <t xml:space="preserve">dsafdsa</t>
   </si>
+  <si>
+    <t xml:space="preserve">NEW NEW NEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdsafdsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdsafdasfdasfdas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW LAST</t>
+  </si>
 </sst>
 </file>
 
@@ -221,13 +233,13 @@
   </sheetPr>
   <dimension ref="A1:Y1149"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A634" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C651" activeCellId="0" sqref="C651"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3590,16 +3602,28 @@
       </c>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A653" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E653" s="0" t="n">
         <v>653</v>
       </c>
+      <c r="G653" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A654" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="E654" s="0" t="n">
         <v>654</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A655" s="0" t="n">
+        <v>12412412512</v>
+      </c>
       <c r="E655" s="0" t="n">
         <v>655</v>
       </c>
@@ -3608,11 +3632,17 @@
       <c r="E656" s="0" t="n">
         <v>656</v>
       </c>
+      <c r="L656" s="0" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E657" s="0" t="n">
         <v>657</v>
       </c>
+      <c r="J657" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E658" s="0" t="n">
@@ -3623,6 +3653,9 @@
       <c r="E659" s="0" t="n">
         <v>659</v>
       </c>
+      <c r="H659" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E660" s="0" t="n">
@@ -6169,6 +6202,9 @@
       </c>
     </row>
     <row r="1149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1149" s="0" t="s">
+        <v>37</v>
+      </c>
       <c r="E1149" s="0" t="n">
         <v>1149</v>
       </c>

</xml_diff>